<commit_message>
Changes to schema are now reflected in the Excel templates and WebFF.py
</commit_message>
<xml_diff>
--- a/XML/Atomistic-Class1/WebFF-Class1-DataTemplate.xlsx
+++ b/XML/Atomistic-Class1/WebFF-Class1-DataTemplate.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Projects\WebFF-Documentation\Atomistic-Class1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Projects\WebFF-Documentation\XML\Atomistic-Class1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0CA24A6E-36CD-4CC3-84BB-1FD7FC8C6D28}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" firstSheet="16" activeTab="19"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="20" r:id="rId1"/>
@@ -56,8 +57,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="KeywordListTab" type="6" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="KeywordListTab" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\png3\Desktop\KeywordListTab.txt">
       <textFields>
         <textField type="text"/>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="266">
   <si>
     <t>Harmonic</t>
   </si>
@@ -274,9 +275,6 @@
     <t>Data Source</t>
   </si>
   <si>
-    <t>Data Scribe (Name)</t>
-  </si>
-  <si>
     <t>» DOI</t>
   </si>
   <si>
@@ -860,12 +858,21 @@
   </si>
   <si>
     <t>RelationTree</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Data Contact (Name)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1184,7 +1191,7 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1289,6 +1296,12 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -1314,7 +1327,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="KeywordListTab_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="KeywordListTab_1" connectionId="1" xr16:uid="{00000000-0016-0000-0200-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1637,14 +1650,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1656,7 +1669,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="30" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="56" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B1" s="56"/>
     </row>
@@ -1666,7 +1679,7 @@
     </row>
     <row r="3" spans="1:2" s="30" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" s="38"/>
     </row>
@@ -1680,67 +1693,82 @@
       </c>
       <c r="B5" s="34"/>
     </row>
-    <row r="6" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+    <row r="6" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="62" t="s">
+        <v>263</v>
+      </c>
+      <c r="B6" s="63"/>
+    </row>
+    <row r="7" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="37"/>
-    </row>
-    <row r="7" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="B7" s="37"/>
+    </row>
+    <row r="8" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="35"/>
-    </row>
-    <row r="8" spans="1:2" ht="133.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="B8" s="35"/>
+    </row>
+    <row r="9" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="B9" s="35"/>
+    </row>
+    <row r="10" spans="1:2" ht="133.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="36"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="B10" s="36"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="37"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="37"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+      <c r="B12" s="37"/>
+    </row>
+    <row r="13" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="37"/>
-    </row>
-    <row r="11" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+      <c r="B13" s="35"/>
+    </row>
+    <row r="14" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>265</v>
+      </c>
+      <c r="B14" s="37"/>
+    </row>
+    <row r="15" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="35"/>
-    </row>
-    <row r="12" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="37"/>
-    </row>
-    <row r="13" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="B15" s="37"/>
+    </row>
+    <row r="16" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="37"/>
-    </row>
-    <row r="14" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" s="49"/>
+      <c r="B16" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B6" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"?, Atomistic - Class I, Atomistic - Class II, Atomistic - Bond Order, Atomistic - ReaxFF, Atomistic - Polarizable, Atomistic - United Atom (UA), Coarse-Grained (CG) - Pseudo-Atom"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{CA8574A2-2C56-4FA8-AE4A-9714A1E7A46C}">
+      <formula1>"Mixed-English,Mixed-Metric,Reduced"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1749,7 +1777,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
@@ -1778,7 +1806,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -1790,7 +1818,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>35</v>
@@ -1802,10 +1830,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -1817,7 +1845,7 @@
         <v>33</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -1848,33 +1876,33 @@
         <v>30</v>
       </c>
       <c r="H8" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="I8" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="J8" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="J8" s="24" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0900-000000000000}">
       <formula1>"?,cis,trans,cis:left,cis:right,trans:left,trans:right"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0900-000001000000}">
       <formula1>"Harmonic"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0900-000002000000}">
       <formula1>"Kd*[1+Ns*cos(N*Phi)]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0900-000003000000}">
       <formula1>"? , kcal, kJ"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G14:G1048576">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G14:G1048576" xr:uid="{00000000-0002-0000-0900-000004000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F14:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F14:F1048576" xr:uid="{00000000-0002-0000-0900-000005000000}">
       <formula1>"-1, 1"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1884,7 +1912,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
@@ -1913,7 +1941,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>37</v>
@@ -1925,7 +1953,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>38</v>
@@ -1937,10 +1965,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -1952,7 +1980,7 @@
         <v>33</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -1992,30 +2020,30 @@
         <v>31</v>
       </c>
       <c r="G9" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="H9" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="I9" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0A00-000000000000}">
       <formula1>"?,cis,trans,cis:left,cis:right,trans:left,trans:right"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0A00-000001000000}">
       <formula1>"Quadratic"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0A00-000002000000}">
       <formula1>"Kd*(Phi-Phi0)^2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0A00-000003000000}">
       <formula1>"? , kcal, kJ"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{00000000-0002-0000-0A00-000004000000}">
       <formula1>"degrees"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2025,7 +2053,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
@@ -2056,7 +2084,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>44</v>
@@ -2068,7 +2096,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>39</v>
@@ -2080,10 +2108,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C5" s="5"/>
       <c r="F5" s="5" t="s">
@@ -2092,10 +2120,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6" s="5"/>
       <c r="F6" s="5" t="s">
@@ -2129,27 +2157,27 @@
         <v>43</v>
       </c>
       <c r="I8" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="J8" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="J8" s="24" t="s">
+      <c r="K8" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="K8" s="24" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0B00-000000000000}">
       <formula1>"? , kcal, kJ"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0B00-000001000000}">
       <formula1>"0.5*{K1*[1+cos(Phi)]+K2*[1-cos(2*Phi)]+K3*[1+cos(3*Phi)]+K4*[1-cos(4*Phi)]}"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0B00-000002000000}">
       <formula1>"OPLS"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0B00-000003000000}">
       <formula1>"?,cis,trans,cis:left,cis:right,trans:left,trans:right"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2159,7 +2187,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
@@ -2189,10 +2217,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C3" s="5"/>
       <c r="G3" s="5" t="s">
@@ -2201,10 +2229,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C4" s="5"/>
       <c r="G4" s="5" t="s">
@@ -2213,10 +2241,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5" s="5"/>
       <c r="G5" s="5" t="s">
@@ -2225,10 +2253,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6" s="5"/>
       <c r="G6" s="5" t="s">
@@ -2261,30 +2289,30 @@
         <v>43</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J8" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="K8" s="45" t="s">
         <v>138</v>
       </c>
-      <c r="K8" s="45" t="s">
+      <c r="L8" s="45" t="s">
         <v>139</v>
-      </c>
-      <c r="L8" s="45" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0C00-000000000000}">
       <formula1>"?,cis,trans,cis:right,cis:left,trans:right,trans:left"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0C00-000001000000}">
       <formula1>"Fourier-Simple"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0C00-000002000000}">
       <formula1>"K1*[1+cos(Phi)]+K2*[1+cos(2*Phi)]+K3*[1+cos(3*Phi)]+K4*[1+cos(4*Phi)]+K5*[1+cos(5*Phi)], K1*[1-cos(Phi)]+K2*[1-cos(2*Phi)]+K3*[1-cos(3*Phi)]+K4*[1-cos(4*Phi)]+K5*[1-cos(5*Phi)]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0C00-000003000000}">
       <formula1>"? , kcal, kJ"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2294,7 +2322,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
@@ -2318,7 +2346,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>58</v>
@@ -2330,10 +2358,10 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C4" s="5"/>
       <c r="I4" s="5" t="s">
@@ -2342,10 +2370,10 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5" s="5"/>
       <c r="I5" s="5" t="s">
@@ -2354,10 +2382,10 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6" s="5"/>
       <c r="I6" s="5" t="s">
@@ -2366,7 +2394,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>10</v>
@@ -2394,73 +2422,73 @@
         <v>40</v>
       </c>
       <c r="F9" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="G9" s="46" t="s">
         <v>145</v>
-      </c>
-      <c r="G9" s="46" t="s">
-        <v>146</v>
       </c>
       <c r="H9" s="46" t="s">
         <v>41</v>
       </c>
       <c r="I9" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="J9" s="46" t="s">
         <v>147</v>
-      </c>
-      <c r="J9" s="46" t="s">
-        <v>148</v>
       </c>
       <c r="K9" s="46" t="s">
         <v>42</v>
       </c>
       <c r="L9" s="46" t="s">
+        <v>148</v>
+      </c>
+      <c r="M9" s="46" t="s">
         <v>149</v>
-      </c>
-      <c r="M9" s="46" t="s">
-        <v>150</v>
       </c>
       <c r="N9" s="46" t="s">
         <v>43</v>
       </c>
       <c r="O9" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="P9" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="P9" s="46" t="s">
+      <c r="Q9" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="R9" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="Q9" s="46" t="s">
-        <v>107</v>
-      </c>
-      <c r="R9" s="46" t="s">
+      <c r="S9" s="46" t="s">
         <v>153</v>
       </c>
-      <c r="S9" s="46" t="s">
-        <v>154</v>
-      </c>
       <c r="T9" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="U9" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="U9" s="47" t="s">
+      <c r="V9" s="47" t="s">
         <v>139</v>
-      </c>
-      <c r="V9" s="47" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{00000000-0002-0000-0D00-000000000000}">
       <formula1>"degrees"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0D00-000001000000}">
       <formula1>"? , kcal, kJ"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0D00-000002000000}">
       <formula1>"?,cis,trans,cis:right,cis:left,trans:right,trans:left"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0D00-000003000000}">
       <formula1>"Fourier"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0D00-000004000000}">
       <formula1>"K1*[1+cos(N1*Phi-D1)]+K2*[1+cos(N2*Phi-D2)]+K3*[1+cos(N3*Phi-D3)]+K4*[1+cos(N4*Phi-D4)]+K5*[1+cos(N5*Phi-D5)], K1*[1-cos(N1*Phi-D1)]+K2*[1-cos(N2*Phi-D2)]+K3*[1-cos(N3*Phi-D3)]+K4*[1-cos(N4*Phi-D4)]+K5*[1-cos(N5*Phi-D5)]"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2469,7 +2497,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
@@ -2513,7 +2541,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>49</v>
@@ -2528,7 +2556,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>50</v>
@@ -2543,10 +2571,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -2561,7 +2589,7 @@
         <v>53</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -2603,13 +2631,13 @@
         <v>30</v>
       </c>
       <c r="H8" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="I8" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="J8" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="J8" s="24" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -2654,22 +2682,22 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F14:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F14:F1048576" xr:uid="{00000000-0002-0000-0E00-000000000000}">
       <formula1>"-1, 1"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G14:G1048576">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G14:G1048576" xr:uid="{00000000-0002-0000-0E00-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0E00-000002000000}">
       <formula1>"? , kcal, kJ"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0E00-000003000000}">
       <formula1>"Ki*[1+Ns*cos(N*Phi)]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0E00-000004000000}">
       <formula1>"CVFF"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0E00-000005000000}">
       <formula1>"?,cis,trans,cis:right,cis:left,trans:right,trans:left"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2679,7 +2707,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
@@ -2720,7 +2748,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>16</v>
@@ -2734,7 +2762,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>52</v>
@@ -2748,10 +2776,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -2765,7 +2793,7 @@
         <v>53</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -2816,13 +2844,13 @@
         <v>55</v>
       </c>
       <c r="G9" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="H9" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="I9" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2857,19 +2885,19 @@
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{00000000-0002-0000-0F00-000000000000}">
       <formula1>"degrees"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0F00-000001000000}">
       <formula1>"? , kcal, kJ"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0F00-000002000000}">
       <formula1>"Ki*cos(Chi-Chi0)^2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0F00-000003000000}">
       <formula1>"cosine/squared"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0F00-000004000000}">
       <formula1>"?,cis,trans,cis:right,cis:left,trans:right,trans:left"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2879,7 +2907,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
@@ -2907,7 +2935,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -2919,7 +2947,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>56</v>
@@ -2931,10 +2959,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -2946,7 +2974,7 @@
         <v>53</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -2986,30 +3014,30 @@
         <v>55</v>
       </c>
       <c r="G9" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="H9" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="I9" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-1000-000000000000}">
       <formula1>"?,cis,trans,cis:right,cis:left,trans:right,trans:left"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-1000-000001000000}">
       <formula1>"Harmonic"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-1000-000002000000}">
       <formula1>"Ki*(Chi-Chi0)^2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-1000-000003000000}">
       <formula1>"? , kcal/degrees^2, kcal/radians^2, kJ/degrees^2, kJ/radians^2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{00000000-0002-0000-1000-000004000000}">
       <formula1>"degrees"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3019,7 +3047,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
@@ -3048,7 +3076,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>58</v>
@@ -3060,7 +3088,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>62</v>
@@ -3072,10 +3100,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5" s="5"/>
       <c r="F5" s="5" t="s">
@@ -3087,7 +3115,7 @@
         <v>53</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6" s="5"/>
       <c r="F6" s="5" t="s">
@@ -3121,27 +3149,27 @@
         <v>61</v>
       </c>
       <c r="I8" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="J8" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="J8" s="24" t="s">
+      <c r="K8" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="K8" s="24" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-1100-000000000000}">
       <formula1>"?,cis,trans,cis:right,cis:left,trans:right,trans:left"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-1100-000001000000}">
       <formula1>"Fourier"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-1100-000002000000}">
       <formula1>"Ki*[C0+C1*cos(w)+C2*cos(2*w)]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-1100-000003000000}">
       <formula1>"? , kcal, kJ"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3151,7 +3179,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
@@ -3180,7 +3208,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>63</v>
@@ -3192,7 +3220,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>64</v>
@@ -3204,10 +3232,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5" s="5"/>
       <c r="G5" s="5" t="s">
@@ -3219,7 +3247,7 @@
         <v>53</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6" s="5"/>
       <c r="G6" s="5" t="s">
@@ -3259,30 +3287,30 @@
         <v>65</v>
       </c>
       <c r="G9" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="H9" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="I9" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{00000000-0002-0000-1200-000000000000}">
       <formula1>"degrees"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-1200-000001000000}">
       <formula1>"? , kcal, kJ"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-1200-000002000000}">
       <formula1>"0.5*K*[{1+cos(w0)}/sin(w0)]^2*[cos(w)-cos(w0)] ~ w0 ≠ 0° &lt;&gt; K*[1-cos(w)] ~ w0 = 0°"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-1200-000003000000}">
       <formula1>"Umbrella"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-1200-000004000000}">
       <formula1>"?,cis,trans,cis:right,cis:left,trans:right,trans:left"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3292,7 +3320,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -3321,7 +3349,7 @@
     </row>
     <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" s="12"/>
     </row>
@@ -3334,7 +3362,7 @@
         <v>48</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3413,7 +3441,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>KeywordsList!$A$1:$A$74</xm:f>
           </x14:formula1>
@@ -3426,13 +3454,13 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -3455,7 +3483,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>18</v>
@@ -3467,22 +3495,22 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -3494,7 +3522,7 @@
         <v>33</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -3537,30 +3565,30 @@
         <v>31</v>
       </c>
       <c r="H9" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="I9" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="J9" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="J9" s="24" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{00000000-0002-0000-1300-000000000000}">
       <formula1>"degrees"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-1300-000001000000}">
       <formula1>"? , kcal, kJ"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-1300-000002000000}">
       <formula1>"?, Kd*[1+cos(N*Phi-Phi0)], Kd*[1+cos(N*Phi+Phi0)], 0.5*Kd*[1+cos(N*Phi-Phi0)], 0.5*Kd*[1+cos(N*Phi+Phi0)]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-1300-000003000000}">
       <formula1>"CHARMM"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-1300-000004000000}">
       <formula1>"?,cis,trans,cis:right,cis:left,trans:right,trans:left"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3569,7 +3597,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
@@ -3590,7 +3618,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -3598,10 +3626,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>12</v>
@@ -3609,10 +3637,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>12</v>
@@ -3620,10 +3648,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -3631,10 +3659,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>24</v>
@@ -3642,10 +3670,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>24</v>
@@ -3654,39 +3682,39 @@
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="C9" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="23" t="s">
-        <v>79</v>
-      </c>
       <c r="D9" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="F9" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-1400-000000000000}">
       <formula1>"?, Å, nm"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-1400-000001000000}">
       <formula1>"?, kcal/mol, kJ/mol"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-1400-000002000000}">
       <formula1>"4*epsilon*[(sigma/R)^12-(sigma/R)^6]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-1400-000003000000}">
       <formula1>"Lennard-Jones (12-6)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{00000000-0002-0000-1400-000004000000}">
       <formula1>"?,Lorentz-Berthelot,Waldman-Hagler,Kong,Fender-Halsey"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3696,7 +3724,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
@@ -3717,7 +3745,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -3725,10 +3753,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>12</v>
@@ -3736,10 +3764,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>12</v>
@@ -3747,10 +3775,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -3758,10 +3786,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>24</v>
@@ -3769,10 +3797,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>24</v>
@@ -3781,39 +3809,39 @@
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="23" t="s">
-        <v>78</v>
-      </c>
       <c r="C9" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D9" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="F9" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{00000000-0002-0000-1500-000000000000}">
       <formula1>"?,Lorentz-Berthelot,Waldman-Hagler,Kong,Fender-Halsey"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-1500-000001000000}">
       <formula1>"Lennard-Jones (12-6) [Rmin Form]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-1500-000002000000}">
       <formula1>"epsilon*[(Rmin/R)^12-2*(Rmin/R)^6]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-1500-000003000000}">
       <formula1>"?,Å,nm"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-1500-000004000000}">
       <formula1>"?,kcal/mol,kJ/mol"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3823,7 +3851,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
@@ -3844,7 +3872,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="56"/>
       <c r="C1" s="56"/>
@@ -3854,10 +3882,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>12</v>
@@ -3865,10 +3893,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>12</v>
@@ -3876,10 +3904,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -3887,10 +3915,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>24</v>
@@ -3898,10 +3926,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>24</v>
@@ -3910,22 +3938,22 @@
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D9" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="F9" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3933,19 +3961,19 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-1600-000000000000}">
       <formula1>"?, kcal*Å^12/mol, kJ*nm^12/mol"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-1600-000001000000}">
       <formula1>"?, kcal*Å^6/mol, kJ*nm^6/mol"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-1600-000002000000}">
       <formula1>"A/(R^12)-B/(R^6)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-1600-000003000000}">
       <formula1>"Lennard-Jones (12-6) [A-B Form]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{00000000-0002-0000-1600-000004000000}">
       <formula1>"?,Lorentz-Berthelot,Waldman-Hagler,Kong,Fender-Halsey"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3955,7 +3983,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
@@ -3976,7 +4004,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -3984,10 +4012,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>12</v>
@@ -3995,10 +4023,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>12</v>
@@ -4006,10 +4034,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -4017,10 +4045,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>24</v>
@@ -4028,10 +4056,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>24</v>
@@ -4040,39 +4068,39 @@
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="C9" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="23" t="s">
-        <v>79</v>
-      </c>
       <c r="D9" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="F9" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{00000000-0002-0000-1700-000000000000}">
       <formula1>"?,Lorentz-Berthelot,Waldman-Hagler,Kong,Fender-Halsey"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-1700-000001000000}">
       <formula1>"Lennard-Jones (9-6) [Class 2 Form]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-1700-000002000000}">
       <formula1>"epsilon*[2*(sigma/R)^9-3*(sigma/R)^6]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-1700-000003000000}">
       <formula1>"?, kcal/mol, kJ/mol"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-1700-000004000000}">
       <formula1>"?, Å, nm"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4082,7 +4110,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
@@ -4104,7 +4132,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="56"/>
       <c r="C1" s="56"/>
@@ -4115,10 +4143,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>12</v>
@@ -4126,10 +4154,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>12</v>
@@ -4137,10 +4165,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -4148,10 +4176,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>24</v>
@@ -4159,10 +4187,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>24</v>
@@ -4177,19 +4205,19 @@
         <v>5</v>
       </c>
       <c r="C9" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="D9" s="23" t="s">
-        <v>79</v>
-      </c>
       <c r="E9" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="F9" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="G9" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -4197,19 +4225,19 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{00000000-0002-0000-1800-000000000000}">
       <formula1>"?,Lorentz-Berthelot,Waldman-Hagler,Kong,Fender-Halsey"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-1800-000001000000}">
       <formula1>"Lennard-Jones (12-6)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-1800-000002000000}">
       <formula1>"4*epsilon*[(sigma/R)^12-(sigma/R)^6]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-1800-000003000000}">
       <formula1>"?, kcal/mol, kJ/mol"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-1800-000004000000}">
       <formula1>"?, Å, nm"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4219,7 +4247,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -4240,7 +4268,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="56"/>
       <c r="C1" s="56"/>
@@ -4253,10 +4281,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" s="58" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C3" s="59"/>
       <c r="D3" s="59"/>
@@ -4269,31 +4297,31 @@
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="D5" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="E5" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="F5" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="F5" s="23" t="s">
-        <v>94</v>
-      </c>
       <c r="G5" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="H5" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="I5" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="I5" s="24" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -4307,7 +4335,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -4334,7 +4362,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="56" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B1" s="56"/>
       <c r="C1" s="56"/>
@@ -4351,10 +4379,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" s="58" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C3" s="59"/>
       <c r="D3" s="59"/>
@@ -4371,43 +4399,43 @@
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="E5" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="E5" s="23" t="s">
+      <c r="F5" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="G5" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="H5" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="I5" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="J5" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="J5" s="23" t="s">
+      <c r="K5" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="K5" s="24" t="s">
+      <c r="L5" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="L5" s="24" t="s">
+      <c r="M5" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="M5" s="24" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -4420,7 +4448,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
@@ -4442,7 +4470,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="56" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B1" s="56"/>
       <c r="C1" s="56"/>
@@ -4455,7 +4483,7 @@
     </row>
     <row r="3" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" s="41"/>
       <c r="C3" s="42"/>
@@ -4467,25 +4495,25 @@
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="C5" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>102</v>
-      </c>
       <c r="E5" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="G5" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -4497,7 +4525,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
@@ -4520,7 +4548,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="56" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1" s="56"/>
       <c r="C1" s="56"/>
@@ -4532,10 +4560,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>12</v>
@@ -4544,39 +4572,39 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" s="53" t="s">
+        <v>251</v>
+      </c>
+      <c r="C6" s="53" t="s">
         <v>252</v>
       </c>
-      <c r="C6" s="53" t="s">
-        <v>253</v>
-      </c>
       <c r="D6" s="52" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E6" s="24" t="s">
         <v>46</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G6" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="H6" s="24" t="s">
         <v>158</v>
-      </c>
-      <c r="H6" s="24" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4634,7 +4662,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-1C00-000000000000}">
       <formula1>"?, ATDL"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4644,7 +4672,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -4695,367 +4723,367 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -5064,7 +5092,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
@@ -5087,7 +5115,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="56" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1" s="56"/>
       <c r="C1" s="56"/>
@@ -5097,10 +5125,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>255</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>256</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>12</v>
@@ -5109,33 +5137,33 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" s="53" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>46</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E6" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="F6" s="24" t="s">
         <v>158</v>
-      </c>
-      <c r="F6" s="24" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -5183,7 +5211,7 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-1D00-000000000000}">
       <formula1>"?, DFF"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5192,7 +5220,7 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
@@ -5215,7 +5243,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="56" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1" s="56"/>
       <c r="C1" s="56"/>
@@ -5225,10 +5253,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>12</v>
@@ -5237,33 +5265,33 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" s="53" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>46</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E6" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="F6" s="24" t="s">
         <v>158</v>
-      </c>
-      <c r="F6" s="24" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -5311,7 +5339,7 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-1E00-000000000000}">
       <formula1>"?, Generic"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5320,7 +5348,7 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
@@ -5346,7 +5374,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -5354,7 +5382,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" s="61"/>
       <c r="C3" s="61"/>
@@ -5367,28 +5395,28 @@
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -5401,7 +5429,7 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
@@ -5428,7 +5456,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -5436,7 +5464,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" s="61"/>
       <c r="C3" s="61"/>
@@ -5450,31 +5478,31 @@
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -5487,7 +5515,7 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
@@ -5506,7 +5534,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="30" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="56" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B1" s="56"/>
     </row>
@@ -5516,7 +5544,7 @@
     </row>
     <row r="3" spans="1:2" s="30" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" s="38"/>
     </row>
@@ -5526,7 +5554,7 @@
     </row>
     <row r="5" spans="1:2" ht="338.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="54" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B5" s="55"/>
     </row>
@@ -5540,7 +5568,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -5585,7 +5613,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -5600,7 +5628,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
@@ -5618,7 +5646,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -5633,7 +5661,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>24</v>
@@ -5666,13 +5694,13 @@
         <v>7</v>
       </c>
       <c r="E8" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="F8" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="G8" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -5680,16 +5708,16 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Harmonic"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"K*(R-R0)^2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>"?, kcal/mol/Å^2, kJ/mol/nm^2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0300-000003000000}">
       <formula1>"?, Å, nm"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5699,7 +5727,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -5736,10 +5764,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>124</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
@@ -5748,10 +5776,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>126</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
@@ -5760,10 +5788,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -5772,10 +5800,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -5787,7 +5815,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
@@ -5805,22 +5833,22 @@
         <v>5</v>
       </c>
       <c r="C9" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="23" t="s">
         <v>128</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>129</v>
       </c>
       <c r="E9" s="23" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="G9" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="H9" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -5828,19 +5856,19 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>"?, 1/Å, 1/nm"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0400-000001000000}">
       <formula1>"? , kcal/mol, kJ/mol"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0400-000002000000}">
       <formula1>"D*[(1-exp(-A(R-R0))]^2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0400-000003000000}">
       <formula1>"Morse"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{00000000-0002-0000-0400-000004000000}">
       <formula1>"?, Å, nm"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5849,7 +5877,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
@@ -5889,7 +5917,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -5900,7 +5928,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>13</v>
@@ -5914,7 +5942,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -5949,16 +5977,16 @@
         <v>15</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G8" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="H8" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="I8" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="I8" s="24" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -5966,16 +5994,16 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>"degrees"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>"?, kcal/mol/degrees^2, kJ/mol/degrees^2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0500-000002000000}">
       <formula1>"Ka*(Theta-Theta0)^2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0500-000003000000}">
       <formula1>"Harmonic"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5985,7 +6013,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
@@ -6025,7 +6053,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>16</v>
@@ -6037,7 +6065,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>17</v>
@@ -6052,7 +6080,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -6089,16 +6117,16 @@
         <v>15</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G8" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="H8" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="I8" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="I8" s="24" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -6106,16 +6134,16 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>"cosine/squared"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0600-000001000000}">
       <formula1>"Ka*[cos(Theta)-cos(Theta0)]^2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0600-000002000000}">
       <formula1>"?,kcal/mol,kJ/mol"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0600-000003000000}">
       <formula1>"degrees"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6125,7 +6153,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
@@ -6165,7 +6193,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>18</v>
@@ -6177,7 +6205,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>19</v>
@@ -6192,7 +6220,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -6216,7 +6244,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
@@ -6228,7 +6256,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
@@ -6261,16 +6289,16 @@
         <v>27</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I10" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="J10" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="J10" s="24" t="s">
+      <c r="K10" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="K10" s="24" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -6278,22 +6306,22 @@
     <mergeCell ref="A1:K1"/>
   </mergeCells>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>"degrees"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0700-000001000000}">
       <formula1>"? , kcal/mol/degrees^2, kJ/mol/degrees^2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0700-000002000000}">
       <formula1>"Ka*(Theta-Theta0)^2+Kub*(R-Rub)^2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0700-000003000000}">
       <formula1>"CHARMM"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{00000000-0002-0000-0700-000004000000}">
       <formula1>"?, kcal/mol/Å^2, kJ/mol/nm^2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{00000000-0002-0000-0700-000005000000}">
       <formula1>"?,Å,nm"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6303,7 +6331,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
@@ -6333,7 +6361,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>18</v>
@@ -6345,22 +6373,22 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -6372,7 +6400,7 @@
         <v>33</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -6415,13 +6443,13 @@
         <v>31</v>
       </c>
       <c r="H9" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="I9" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="J9" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="J9" s="24" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -6441,19 +6469,19 @@
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"degrees"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>"? , kcal, kJ"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0800-000002000000}">
       <formula1>"?,Kd*[1+cos(N*Phi-Phi0)]"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"CHARMM"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0800-000004000000}">
       <formula1>"?,cis,trans,cis:right,cis:left,trans:right,trans:left"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added additional enumeration to Dihedral Style CHARMM for the XML schema and Excel Data Template
</commit_message>
<xml_diff>
--- a/XML/Atomistic-Class1/WebFF-Class1-DataTemplate.xlsx
+++ b/XML/Atomistic-Class1/WebFF-Class1-DataTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Projects\WebFF-Documentation\XML\Atomistic-Class1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Projects\WebFF-Documentation\XML\Atomistic-Class1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0CA24A6E-36CD-4CC3-84BB-1FD7FC8C6D28}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DFB5C83F-63A8-4AE3-92A8-B67300FC3230}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="20" r:id="rId1"/>
@@ -1278,6 +1278,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1295,12 +1301,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1656,104 +1656,104 @@
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="31" customWidth="1"/>
+    <col min="1" max="1" width="18.59765625" style="31" customWidth="1"/>
     <col min="2" max="2" width="52" style="31" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="31"/>
+    <col min="3" max="16384" width="9.1328125" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="30" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:2" s="30" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A1" s="58" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="56"/>
-    </row>
-    <row r="2" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="58"/>
+    </row>
+    <row r="2" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="13"/>
       <c r="B2"/>
     </row>
-    <row r="3" spans="1:2" s="30" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="30" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="22" t="s">
         <v>96</v>
       </c>
       <c r="B3" s="38"/>
     </row>
-    <row r="4" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="14"/>
       <c r="B4" s="18"/>
     </row>
-    <row r="5" spans="1:2" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A5" s="32" t="s">
         <v>47</v>
       </c>
       <c r="B5" s="34"/>
     </row>
-    <row r="6" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="62" t="s">
+    <row r="6" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="56" t="s">
         <v>263</v>
       </c>
-      <c r="B6" s="63"/>
-    </row>
-    <row r="7" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="57"/>
+    </row>
+    <row r="7" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="26" t="s">
         <v>45</v>
       </c>
       <c r="B7" s="37"/>
     </row>
-    <row r="8" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="26" t="s">
         <v>46</v>
       </c>
       <c r="B8" s="35"/>
     </row>
-    <row r="9" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="26" t="s">
         <v>264</v>
       </c>
       <c r="B9" s="35"/>
     </row>
-    <row r="10" spans="1:2" ht="133.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="133.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="26" t="s">
         <v>67</v>
       </c>
       <c r="B10" s="36"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="33" t="s">
         <v>68</v>
       </c>
       <c r="B11" s="37"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="33" t="s">
         <v>69</v>
       </c>
       <c r="B12" s="37"/>
     </row>
-    <row r="13" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="33" t="s">
         <v>70</v>
       </c>
       <c r="B13" s="35"/>
     </row>
-    <row r="14" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="28" t="s">
         <v>265</v>
       </c>
       <c r="B14" s="37"/>
     </row>
-    <row r="15" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="28" t="s">
         <v>71</v>
       </c>
       <c r="B15" s="37"/>
     </row>
-    <row r="16" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="28" t="s">
         <v>72</v>
       </c>
@@ -1785,26 +1785,26 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J25" sqref="A9:J25"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.1328125" customWidth="1"/>
+    <col min="8" max="8" width="34.3984375" customWidth="1"/>
+    <col min="9" max="9" width="10.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>122</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>124</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>141</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -1852,8 +1852,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="8" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -1920,26 +1920,26 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K27" sqref="A10:K27"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.1328125" customWidth="1"/>
+    <col min="7" max="7" width="34.3984375" customWidth="1"/>
+    <col min="8" max="8" width="10.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>122</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>124</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>141</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
@@ -1999,8 +1999,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -2064,25 +2064,25 @@
       <selection pane="bottomLeft" activeCell="I32" sqref="A9:I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
+    <col min="3" max="3" width="17.86328125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="34.42578125" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.1328125" customWidth="1"/>
+    <col min="9" max="9" width="34.3984375" customWidth="1"/>
+    <col min="10" max="10" width="10.73046875" customWidth="1"/>
+    <col min="11" max="11" width="9.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>122</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>124</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>141</v>
       </c>
@@ -2118,7 +2118,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>142</v>
       </c>
@@ -2130,8 +2130,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="8" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -2198,24 +2198,24 @@
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
+    <col min="3" max="3" width="17.86328125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="7" width="18" customWidth="1"/>
-    <col min="8" max="9" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="34.42578125" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="8" max="9" width="16.1328125" customWidth="1"/>
+    <col min="10" max="10" width="34.3984375" customWidth="1"/>
+    <col min="11" max="11" width="10.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>122</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>124</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>141</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>142</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2329,22 +2329,22 @@
   <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A10:T23"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="19" width="16.28515625" customWidth="1"/>
-    <col min="20" max="20" width="33.7109375" customWidth="1"/>
-    <col min="21" max="22" width="10.7109375" customWidth="1"/>
+    <col min="1" max="19" width="16.265625" customWidth="1"/>
+    <col min="20" max="20" width="33.73046875" customWidth="1"/>
+    <col min="21" max="22" width="10.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:22" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>122</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>124</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>141</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>142</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>154</v>
       </c>
@@ -2404,8 +2404,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:22" s="48" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:22" s="48" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="46" t="s">
         <v>4</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:22" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{00000000-0002-0000-0D00-000000000000}">
@@ -2508,18 +2508,18 @@
       <selection pane="bottomLeft" activeCell="M29" sqref="A9:M29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" style="7" customWidth="1"/>
     <col min="3" max="4" width="16" style="7" customWidth="1"/>
     <col min="5" max="5" width="18" style="6" customWidth="1"/>
     <col min="6" max="6" width="18" style="8" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.1328125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="34.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -2530,7 +2530,7 @@
       <c r="F1"/>
       <c r="G1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -2539,7 +2539,7 @@
       <c r="F2"/>
       <c r="G2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>122</v>
       </c>
@@ -2554,7 +2554,7 @@
       <c r="F3"/>
       <c r="G3"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>124</v>
       </c>
@@ -2569,7 +2569,7 @@
       <c r="F4"/>
       <c r="G4"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>141</v>
       </c>
@@ -2584,7 +2584,7 @@
       <c r="F5"/>
       <c r="G5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -2599,7 +2599,7 @@
       <c r="F6"/>
       <c r="G6"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7"/>
@@ -2608,7 +2608,7 @@
       <c r="F7"/>
       <c r="G7"/>
     </row>
-    <row r="8" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="50"/>
       <c r="B9" s="50"/>
       <c r="C9" s="50"/>
@@ -2648,7 +2648,7 @@
       <c r="F9" s="50"/>
       <c r="G9" s="50"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="50"/>
       <c r="B10" s="50"/>
       <c r="C10" s="50"/>
@@ -2656,7 +2656,7 @@
       <c r="F10" s="50"/>
       <c r="G10" s="50"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="50"/>
       <c r="B11" s="50"/>
       <c r="C11" s="50"/>
@@ -2664,7 +2664,7 @@
       <c r="F11" s="50"/>
       <c r="G11" s="50"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="50"/>
       <c r="B12" s="50"/>
       <c r="C12" s="50"/>
@@ -2672,7 +2672,7 @@
       <c r="F12" s="50"/>
       <c r="G12" s="50"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="50"/>
       <c r="B13" s="50"/>
       <c r="C13" s="50"/>
@@ -2718,17 +2718,17 @@
       <selection pane="bottomLeft" activeCell="L33" sqref="A10:L33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" style="7" customWidth="1"/>
     <col min="3" max="4" width="16" style="7" customWidth="1"/>
     <col min="5" max="5" width="18" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.1328125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="34.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -2738,7 +2738,7 @@
       <c r="E1"/>
       <c r="F1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -2746,7 +2746,7 @@
       <c r="E2"/>
       <c r="F2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>122</v>
       </c>
@@ -2760,7 +2760,7 @@
       <c r="E3"/>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>124</v>
       </c>
@@ -2774,7 +2774,7 @@
       <c r="E4"/>
       <c r="F4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>141</v>
       </c>
@@ -2788,7 +2788,7 @@
       <c r="E5"/>
       <c r="F5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -2802,7 +2802,7 @@
       <c r="E6"/>
       <c r="F6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>54</v>
       </c>
@@ -2816,7 +2816,7 @@
       <c r="E7"/>
       <c r="F7"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
@@ -2824,7 +2824,7 @@
       <c r="E8"/>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -2853,31 +2853,31 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="50"/>
       <c r="B10" s="50"/>
       <c r="C10" s="50"/>
       <c r="D10" s="50"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="50"/>
       <c r="B11" s="50"/>
       <c r="C11" s="50"/>
       <c r="D11" s="50"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="50"/>
       <c r="B12" s="50"/>
       <c r="C12" s="50"/>
       <c r="D12" s="50"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="50"/>
       <c r="B13" s="50"/>
       <c r="C13" s="50"/>
       <c r="D13" s="50"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="50"/>
       <c r="B14" s="50"/>
       <c r="C14" s="50"/>
@@ -2918,22 +2918,22 @@
       <selection pane="bottomLeft" activeCell="M35" sqref="A10:M35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.1328125" customWidth="1"/>
+    <col min="7" max="7" width="34.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>122</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>124</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>141</v>
       </c>
@@ -2969,7 +2969,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>54</v>
       </c>
@@ -2993,8 +2993,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -3058,23 +3058,23 @@
       <selection pane="bottomLeft" activeCell="I33" sqref="A9:I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
+    <col min="3" max="3" width="17.86328125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="34.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.1328125" customWidth="1"/>
+    <col min="9" max="9" width="34.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>122</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>124</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>141</v>
       </c>
@@ -3110,7 +3110,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -3122,8 +3122,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="8" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -3190,23 +3190,23 @@
       <selection pane="bottomLeft" activeCell="K29" sqref="A10:K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="35.5703125" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.1328125" customWidth="1"/>
+    <col min="7" max="7" width="35.59765625" customWidth="1"/>
+    <col min="8" max="8" width="10.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>122</v>
       </c>
@@ -3218,7 +3218,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>124</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>141</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -3254,7 +3254,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>66</v>
       </c>
@@ -3266,8 +3266,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -3331,33 +3331,33 @@
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="43.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.1328125" customWidth="1"/>
+    <col min="2" max="2" width="43.1328125" customWidth="1"/>
     <col min="3" max="16384" width="9" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="57"/>
-    </row>
-    <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="59"/>
+    </row>
+    <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="13"/>
     </row>
-    <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="22" t="s">
         <v>96</v>
       </c>
       <c r="B3" s="12"/>
     </row>
-    <row r="4" spans="1:2" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="14"/>
       <c r="B4" s="18"/>
     </row>
-    <row r="5" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="23" t="s">
         <v>48</v>
       </c>
@@ -3365,71 +3365,71 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="19"/>
       <c r="B6" s="19"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="19"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="19"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="19"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="19"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="19"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="19"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="19"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="19"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="19"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="19"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="19"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="19"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="19"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="19"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="19"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" s="19"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" s="19"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" s="19"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" s="19"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" s="19"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" s="19"/>
     </row>
   </sheetData>
@@ -3464,24 +3464,24 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.1328125" customWidth="1"/>
+    <col min="8" max="8" width="34.3984375" customWidth="1"/>
+    <col min="9" max="9" width="10.73046875" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>122</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>124</v>
       </c>
@@ -3505,7 +3505,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>141</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
@@ -3541,8 +3541,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -3608,15 +3608,15 @@
       <selection pane="bottomLeft" activeCell="H23" sqref="A10:H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" customWidth="1"/>
+    <col min="2" max="2" width="35.86328125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="36.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="10" t="s">
         <v>73</v>
       </c>
@@ -3624,7 +3624,7 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>122</v>
       </c>
@@ -3635,7 +3635,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>124</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>81</v>
       </c>
@@ -3657,7 +3657,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>82</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>155</v>
       </c>
@@ -3679,8 +3679,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>76</v>
       </c>
@@ -3735,15 +3735,15 @@
       <selection pane="bottomLeft" activeCell="I37" sqref="A10:I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.86328125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="36.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="10" t="s">
         <v>73</v>
       </c>
@@ -3751,7 +3751,7 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>122</v>
       </c>
@@ -3762,7 +3762,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>124</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>81</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>83</v>
       </c>
@@ -3795,7 +3795,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>155</v>
       </c>
@@ -3806,8 +3806,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>76</v>
       </c>
@@ -3862,25 +3862,25 @@
       <selection pane="bottomLeft" activeCell="J35" sqref="A10:J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.86328125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="36.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:6" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>122</v>
       </c>
@@ -3891,7 +3891,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>124</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>85</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>87</v>
       </c>
@@ -3924,7 +3924,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>155</v>
       </c>
@@ -3935,8 +3935,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>76</v>
       </c>
@@ -3994,15 +3994,15 @@
       <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.3984375" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="36.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="10" t="s">
         <v>73</v>
       </c>
@@ -4010,7 +4010,7 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>122</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>124</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>81</v>
       </c>
@@ -4043,7 +4043,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>82</v>
       </c>
@@ -4054,7 +4054,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>155</v>
       </c>
@@ -4065,8 +4065,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>76</v>
       </c>
@@ -4121,27 +4121,27 @@
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.73046875" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.59765625" customWidth="1"/>
+    <col min="5" max="5" width="33.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:7" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>122</v>
       </c>
@@ -4152,7 +4152,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>124</v>
       </c>
@@ -4163,7 +4163,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>81</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>82</v>
       </c>
@@ -4185,7 +4185,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>155</v>
       </c>
@@ -4196,8 +4196,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -4257,45 +4257,45 @@
       <selection activeCell="L35" sqref="A6:L35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.1328125" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" customWidth="1"/>
+    <col min="7" max="7" width="26.265625" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="60"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="62"/>
+    </row>
+    <row r="4" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="5" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="23" t="s">
         <v>76</v>
       </c>
@@ -4345,59 +4345,59 @@
       <selection activeCell="K30" sqref="A6:K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="9" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" customWidth="1"/>
-    <col min="11" max="11" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.1328125" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" customWidth="1"/>
+    <col min="3" max="3" width="15.1328125" customWidth="1"/>
+    <col min="5" max="5" width="10.3984375" customWidth="1"/>
+    <col min="6" max="6" width="11.265625" customWidth="1"/>
+    <col min="7" max="7" width="12.1328125" customWidth="1"/>
+    <col min="8" max="9" width="15.73046875" customWidth="1"/>
+    <col min="10" max="10" width="18.1328125" customWidth="1"/>
+    <col min="11" max="11" width="26.265625" customWidth="1"/>
     <col min="12" max="12" width="11" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="13" max="13" width="16.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:13" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="58" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="60"/>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="62"/>
+    </row>
+    <row r="4" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="5" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="23" t="s">
         <v>76</v>
       </c>
@@ -4458,30 +4458,30 @@
       <selection activeCell="M34" sqref="A6:M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.86328125" customWidth="1"/>
+    <col min="3" max="3" width="10.1328125" customWidth="1"/>
+    <col min="4" max="4" width="9.73046875" customWidth="1"/>
+    <col min="5" max="5" width="22.265625" customWidth="1"/>
+    <col min="6" max="6" width="11.3984375" customWidth="1"/>
+    <col min="7" max="7" width="15.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="58" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
     </row>
-    <row r="3" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>96</v>
       </c>
@@ -4492,8 +4492,8 @@
       <c r="F3" s="42"/>
       <c r="G3" s="43"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="5" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="23" t="s">
         <v>99</v>
       </c>
@@ -4535,30 +4535,30 @@
       <selection sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.73046875" customWidth="1"/>
+    <col min="2" max="2" width="37.3984375" customWidth="1"/>
     <col min="3" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="44"/>
+    <col min="5" max="5" width="35.265625" customWidth="1"/>
+    <col min="7" max="7" width="15.73046875" customWidth="1"/>
+    <col min="8" max="8" width="12.3984375" customWidth="1"/>
+    <col min="9" max="16384" width="9.1328125" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:8" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>254</v>
       </c>
@@ -4570,7 +4570,7 @@
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>137</v>
       </c>
@@ -4580,8 +4580,8 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="6" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="23" t="s">
         <v>110</v>
       </c>
@@ -4607,7 +4607,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="51"/>
       <c r="B7" s="51"/>
       <c r="C7" s="51"/>
@@ -4617,7 +4617,7 @@
       <c r="G7" s="51"/>
       <c r="H7" s="51"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="51"/>
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
@@ -4627,7 +4627,7 @@
       <c r="G8" s="51"/>
       <c r="H8" s="51"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="51"/>
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
@@ -4637,7 +4637,7 @@
       <c r="G9" s="51"/>
       <c r="H9" s="51"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="51"/>
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
@@ -4647,7 +4647,7 @@
       <c r="G10" s="51"/>
       <c r="H10" s="51"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="51"/>
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
@@ -4682,406 +4682,406 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="31" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="37" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="31" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="23.86328125" bestFit="1" customWidth="1"/>
+    <col min="33" max="37" width="8.3984375" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="14" bestFit="1" customWidth="1"/>
-    <col min="39" max="44" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="58" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="60" max="61" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="44" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="46" max="58" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.73046875" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="7" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="70" max="72" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="25.86328125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="6.3984375" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="70" max="72" width="8.3984375" bestFit="1" customWidth="1"/>
     <col min="73" max="73" width="25" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="9.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="7" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" s="7" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" s="7" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" s="7" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" s="7" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" s="7" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" s="7" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" s="7" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" s="7" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" s="7" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="7" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="7" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="7" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" s="7" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" s="7" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" s="7" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" s="7" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" s="7" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" s="7" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" s="7" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" s="7" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" s="7" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" s="7" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" s="7" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" s="7" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" s="7" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" s="7" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" s="7" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A37" s="7" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38" s="7" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39" s="7" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A40" s="7" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A41" s="7" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42" s="7" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43" s="7" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A44" s="7" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A45" s="7" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A46" s="7" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A47" s="7" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A48" s="7" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A49" s="7" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50" s="7" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A51" s="7" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A52" s="7" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A53" s="7" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A54" s="7" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A55" s="7" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A56" s="7" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A57" s="7" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A58" s="7" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A59" s="7" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A60" s="7" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A61" s="7" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A62" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A63" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A64" s="7" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A65" s="7" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A66" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A67" s="7" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A68" s="7" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A69" s="7" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A70" s="7" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A71" s="7" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A72" s="7" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A73" s="7" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A74" s="7" t="s">
         <v>192</v>
       </c>
@@ -5102,28 +5102,28 @@
       <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.73046875" customWidth="1"/>
+    <col min="2" max="2" width="37.3984375" customWidth="1"/>
+    <col min="3" max="3" width="32.73046875" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="44"/>
+    <col min="5" max="5" width="16.73046875" customWidth="1"/>
+    <col min="6" max="6" width="12.3984375" customWidth="1"/>
+    <col min="7" max="16384" width="9.1328125" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:6" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>254</v>
       </c>
@@ -5135,7 +5135,7 @@
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>137</v>
       </c>
@@ -5145,8 +5145,8 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="6" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="23" t="s">
         <v>110</v>
       </c>
@@ -5166,7 +5166,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="51"/>
       <c r="B7" s="51"/>
       <c r="C7" s="51"/>
@@ -5174,7 +5174,7 @@
       <c r="E7" s="51"/>
       <c r="F7" s="51"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="51"/>
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
@@ -5182,7 +5182,7 @@
       <c r="E8" s="51"/>
       <c r="F8" s="51"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="51"/>
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
@@ -5190,7 +5190,7 @@
       <c r="E9" s="51"/>
       <c r="F9" s="51"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="51"/>
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
@@ -5198,7 +5198,7 @@
       <c r="E10" s="51"/>
       <c r="F10" s="51"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="51"/>
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
@@ -5230,28 +5230,28 @@
       <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.73046875" customWidth="1"/>
+    <col min="2" max="2" width="37.3984375" customWidth="1"/>
+    <col min="3" max="3" width="32.73046875" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="44"/>
+    <col min="5" max="5" width="16.73046875" customWidth="1"/>
+    <col min="6" max="6" width="12.3984375" customWidth="1"/>
+    <col min="7" max="16384" width="9.1328125" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:6" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>254</v>
       </c>
@@ -5263,7 +5263,7 @@
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>137</v>
       </c>
@@ -5273,8 +5273,8 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="6" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="23" t="s">
         <v>110</v>
       </c>
@@ -5294,7 +5294,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="51"/>
       <c r="B7" s="51"/>
       <c r="C7" s="51"/>
@@ -5302,7 +5302,7 @@
       <c r="E7" s="51"/>
       <c r="F7" s="51"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="51"/>
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
@@ -5310,7 +5310,7 @@
       <c r="E8" s="51"/>
       <c r="F8" s="51"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="51"/>
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
@@ -5318,7 +5318,7 @@
       <c r="E9" s="51"/>
       <c r="F9" s="51"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="51"/>
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
@@ -5326,7 +5326,7 @@
       <c r="E10" s="51"/>
       <c r="F10" s="51"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="51"/>
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
@@ -5359,20 +5359,20 @@
       <selection pane="bottomLeft" sqref="A1:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.1328125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.59765625" customWidth="1"/>
+    <col min="7" max="7" width="17.1328125" customWidth="1"/>
+    <col min="8" max="8" width="17.73046875" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="10" t="s">
         <v>260</v>
       </c>
@@ -5380,20 +5380,20 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+    </row>
+    <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="5" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="23" t="s">
         <v>110</v>
       </c>
@@ -5440,21 +5440,21 @@
       <selection pane="bottomLeft" sqref="A1:I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.1328125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.59765625" customWidth="1"/>
+    <col min="7" max="7" width="13.3984375" customWidth="1"/>
+    <col min="8" max="8" width="17.1328125" customWidth="1"/>
+    <col min="9" max="9" width="17.73046875" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="10" t="s">
         <v>259</v>
       </c>
@@ -5462,21 +5462,21 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+    </row>
+    <row r="4" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="5" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="23" t="s">
         <v>110</v>
       </c>
@@ -5525,34 +5525,34 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="31" customWidth="1"/>
+    <col min="1" max="1" width="18.59765625" style="31" customWidth="1"/>
     <col min="2" max="2" width="52" style="31" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="31"/>
+    <col min="3" max="16384" width="9.1328125" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="30" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:2" s="30" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A1" s="58" t="s">
         <v>261</v>
       </c>
-      <c r="B1" s="56"/>
-    </row>
-    <row r="2" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="58"/>
+    </row>
+    <row r="2" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="13"/>
       <c r="B2"/>
     </row>
-    <row r="3" spans="1:2" s="30" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="30" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="22" t="s">
         <v>96</v>
       </c>
       <c r="B3" s="38"/>
     </row>
-    <row r="4" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="14"/>
       <c r="B4" s="18"/>
     </row>
-    <row r="5" spans="1:2" ht="338.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="338.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A5" s="54" t="s">
         <v>262</v>
       </c>
@@ -5579,30 +5579,30 @@
       <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.73046875" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="40"/>
+    <col min="4" max="4" width="16.1328125" customWidth="1"/>
+    <col min="5" max="5" width="36.1328125" customWidth="1"/>
+    <col min="6" max="6" width="9.73046875" customWidth="1"/>
+    <col min="7" max="7" width="10.3984375" customWidth="1"/>
+    <col min="8" max="16384" width="9.1328125" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:7" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -5611,7 +5611,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>122</v>
       </c>
@@ -5626,7 +5626,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>124</v>
       </c>
@@ -5641,7 +5641,7 @@
       <c r="F4" s="15"/>
       <c r="G4" s="16"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -5656,7 +5656,7 @@
       <c r="F5" s="15"/>
       <c r="G5" s="16"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -5671,7 +5671,7 @@
       <c r="F6" s="15"/>
       <c r="G6" s="16"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="20"/>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -5680,7 +5680,7 @@
       <c r="F7" s="20"/>
       <c r="G7" s="21"/>
     </row>
-    <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -5737,32 +5737,32 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.86328125" customWidth="1"/>
+    <col min="2" max="2" width="22.86328125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="34.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.1328125" customWidth="1"/>
+    <col min="6" max="6" width="34.3984375" customWidth="1"/>
     <col min="7" max="7" width="9"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="39"/>
+    <col min="8" max="8" width="10.1328125" customWidth="1"/>
+    <col min="9" max="16384" width="9.1328125" style="39"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:8" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>122</v>
       </c>
@@ -5774,7 +5774,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>124</v>
       </c>
@@ -5786,7 +5786,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>126</v>
       </c>
@@ -5798,7 +5798,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>85</v>
       </c>
@@ -5810,7 +5810,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -5822,10 +5822,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -5888,34 +5888,34 @@
       <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.73046875" customWidth="1"/>
+    <col min="2" max="2" width="20.265625" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="25"/>
+    <col min="5" max="5" width="16.1328125" customWidth="1"/>
+    <col min="6" max="6" width="14.3984375" customWidth="1"/>
+    <col min="7" max="7" width="31.3984375" customWidth="1"/>
+    <col min="8" max="8" width="11.1328125" customWidth="1"/>
+    <col min="9" max="9" width="11.265625" customWidth="1"/>
+    <col min="10" max="16384" width="9.1328125" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>122</v>
       </c>
@@ -5926,7 +5926,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>124</v>
       </c>
@@ -5937,7 +5937,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -5948,7 +5948,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -5959,8 +5959,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="8" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -6024,34 +6024,34 @@
       <selection pane="bottomLeft" activeCell="G32" sqref="A9:G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="27"/>
+    <col min="5" max="5" width="16.1328125" customWidth="1"/>
+    <col min="6" max="6" width="11.1328125" customWidth="1"/>
+    <col min="7" max="7" width="34.3984375" customWidth="1"/>
+    <col min="8" max="8" width="10.73046875" customWidth="1"/>
+    <col min="9" max="9" width="15.1328125" customWidth="1"/>
+    <col min="10" max="16384" width="9.1328125" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>122</v>
       </c>
@@ -6063,7 +6063,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>124</v>
       </c>
@@ -6075,7 +6075,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -6087,7 +6087,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -6099,8 +6099,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="8" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -6164,34 +6164,34 @@
       <selection pane="bottomLeft" activeCell="H27" sqref="A11:H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1"/>
-    <col min="9" max="9" width="34.42578125" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
+    <col min="5" max="7" width="16.1328125" customWidth="1"/>
+    <col min="8" max="8" width="11.86328125" customWidth="1"/>
+    <col min="9" max="9" width="34.3984375" customWidth="1"/>
+    <col min="11" max="11" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:11" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>122</v>
       </c>
@@ -6203,7 +6203,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>124</v>
       </c>
@@ -6215,7 +6215,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -6227,7 +6227,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -6239,7 +6239,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -6251,7 +6251,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -6263,10 +6263,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="23" t="s">
         <v>4</v>
       </c>
@@ -6337,29 +6337,29 @@
   </sheetPr>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H33" sqref="A10:H33"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.1328125" customWidth="1"/>
+    <col min="8" max="8" width="34.3984375" customWidth="1"/>
+    <col min="9" max="9" width="10.73046875" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>122</v>
       </c>
@@ -6371,7 +6371,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>124</v>
       </c>
@@ -6383,7 +6383,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>141</v>
       </c>
@@ -6395,7 +6395,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -6407,7 +6407,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
@@ -6419,8 +6419,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -6452,19 +6452,19 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F14" s="8"/>
     </row>
   </sheetData>
@@ -6476,7 +6476,7 @@
       <formula1>"? , kcal, kJ"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0800-000002000000}">
-      <formula1>"?,Kd*[1+cos(N*Phi-Phi0)]"</formula1>
+      <formula1>"?,Kd*[1+cos(N*Phi-Phi0)],Kd*[1+cos(N*Phi+Phi0)]"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"CHARMM"</formula1>

</xml_diff>

<commit_message>
Began addition of comments, and required font changes
</commit_message>
<xml_diff>
--- a/XML/Atomistic-Class1/WebFF-Class1-DataTemplate.xlsx
+++ b/XML/Atomistic-Class1/WebFF-Class1-DataTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Projects\WebFF-Documentation\XML\Atomistic-Class1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Projects\WebFF-Documentation\XML\Atomistic-Class1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{11DCECAA-A73A-47A3-86FA-8BF2250F5110}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E44D4A-0A8F-4BE7-89D3-779322C58314}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="44" r:id="rId1"/>
@@ -57,6 +57,30 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Phelan Jr., Frederick R. Dr. (Fed)</author>
+  </authors>
+  <commentList>
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{44D0F1CD-C13E-4463-8DD3-AEF7DD325C5C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Optional entry, not required
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="KeywordListTab" type="6" refreshedVersion="6" background="1" saveData="1">
@@ -892,7 +916,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -963,15 +987,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1256,9 +1287,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1287,7 +1315,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1300,35 +1327,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1348,6 +1348,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -1696,118 +1727,118 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C880D64F-9BE3-491D-AC61-6F09A4F3CD8E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C880D64F-9BE3-491D-AC61-6F09A4F3CD8E}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="31" customWidth="1"/>
-    <col min="2" max="2" width="75.7109375" style="31" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="31"/>
+    <col min="1" max="1" width="18.59765625" style="31" customWidth="1"/>
+    <col min="2" max="2" width="75.73046875" style="31" customWidth="1"/>
+    <col min="3" max="16384" width="9.1328125" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="30" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:2" s="30" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A1" s="62" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="57"/>
-    </row>
-    <row r="2" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="62"/>
+    </row>
+    <row r="2" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="13"/>
       <c r="B2"/>
     </row>
-    <row r="3" spans="1:2" s="30" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="30" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="37"/>
-    </row>
-    <row r="4" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="36"/>
+    </row>
+    <row r="4" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="14"/>
       <c r="B4" s="18"/>
     </row>
-    <row r="5" spans="1:2" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A5" s="32" t="s">
         <v>264</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="55" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
+    <row r="6" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="53" t="s">
         <v>266</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="54" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="36"/>
-    </row>
-    <row r="8" spans="1:2" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="35"/>
+    </row>
+    <row r="8" spans="1:2" ht="56.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="34"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="33"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="26" t="s">
         <v>262</v>
       </c>
-      <c r="B9" s="34"/>
-    </row>
-    <row r="10" spans="1:2" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="33"/>
+    </row>
+    <row r="10" spans="1:2" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="35"/>
-    </row>
-    <row r="11" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+      <c r="B10" s="34"/>
+    </row>
+    <row r="11" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="36"/>
-    </row>
-    <row r="12" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
+      <c r="B11" s="35"/>
+    </row>
+    <row r="12" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="48"/>
-    </row>
-    <row r="13" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+      <c r="B12" s="47"/>
+    </row>
+    <row r="13" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="34"/>
-    </row>
-    <row r="14" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="33"/>
+    </row>
+    <row r="14" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="28" t="s">
         <v>263</v>
       </c>
-      <c r="B14" s="36"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="35"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="36"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="35"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="48"/>
+      <c r="B16" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1826,6 +1857,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1841,24 +1873,24 @@
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.1328125" customWidth="1"/>
+    <col min="8" max="8" width="34.3984375" customWidth="1"/>
+    <col min="9" max="9" width="10.73046875" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>121</v>
       </c>
@@ -1870,7 +1902,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -1882,7 +1914,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>140</v>
       </c>
@@ -1894,7 +1926,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -1906,7 +1938,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
@@ -1918,8 +1950,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -1951,19 +1983,19 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F14" s="8"/>
     </row>
   </sheetData>
@@ -2001,23 +2033,23 @@
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.1328125" customWidth="1"/>
+    <col min="8" max="8" width="34.3984375" customWidth="1"/>
+    <col min="9" max="9" width="10.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>121</v>
       </c>
@@ -2029,7 +2061,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -2041,7 +2073,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>140</v>
       </c>
@@ -2053,7 +2085,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -2065,8 +2097,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="8" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -2136,23 +2168,23 @@
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.1328125" customWidth="1"/>
+    <col min="7" max="7" width="34.3984375" customWidth="1"/>
+    <col min="8" max="8" width="10.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>121</v>
       </c>
@@ -2164,7 +2196,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -2176,7 +2208,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>140</v>
       </c>
@@ -2188,7 +2220,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -2200,7 +2232,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
@@ -2212,8 +2244,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -2277,25 +2309,25 @@
       <selection pane="bottomLeft" activeCell="I32" sqref="A9:I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
+    <col min="3" max="3" width="17.86328125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="34.42578125" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.1328125" customWidth="1"/>
+    <col min="9" max="9" width="34.3984375" customWidth="1"/>
+    <col min="10" max="10" width="10.73046875" customWidth="1"/>
+    <col min="11" max="11" width="9.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>121</v>
       </c>
@@ -2307,7 +2339,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -2319,7 +2351,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>140</v>
       </c>
@@ -2331,7 +2363,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>141</v>
       </c>
@@ -2343,8 +2375,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="8" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -2411,24 +2443,24 @@
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
+    <col min="3" max="3" width="17.86328125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="7" width="18" customWidth="1"/>
-    <col min="8" max="9" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="34.42578125" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="8" max="9" width="16.1328125" customWidth="1"/>
+    <col min="10" max="10" width="34.3984375" customWidth="1"/>
+    <col min="11" max="11" width="10.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>121</v>
       </c>
@@ -2440,7 +2472,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -2452,7 +2484,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>140</v>
       </c>
@@ -2464,7 +2496,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>141</v>
       </c>
@@ -2476,7 +2508,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2504,13 +2536,13 @@
       <c r="I8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="J8" s="44" t="s">
+      <c r="J8" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="K8" s="44" t="s">
+      <c r="K8" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="L8" s="44" t="s">
+      <c r="L8" s="43" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2545,19 +2577,19 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="19" width="16.28515625" customWidth="1"/>
-    <col min="20" max="20" width="33.7109375" customWidth="1"/>
-    <col min="21" max="22" width="10.7109375" customWidth="1"/>
+    <col min="1" max="19" width="16.265625" customWidth="1"/>
+    <col min="20" max="20" width="33.73046875" customWidth="1"/>
+    <col min="21" max="22" width="10.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:22" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>121</v>
       </c>
@@ -2569,7 +2601,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -2581,7 +2613,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>140</v>
       </c>
@@ -2593,7 +2625,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>141</v>
       </c>
@@ -2605,7 +2637,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>153</v>
       </c>
@@ -2617,76 +2649,76 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:22" s="47" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="45" t="s">
+    <row r="8" spans="1:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:22" s="46" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="D9" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="45" t="s">
+      <c r="F9" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="G9" s="45" t="s">
+      <c r="G9" s="44" t="s">
         <v>144</v>
       </c>
-      <c r="H9" s="45" t="s">
+      <c r="H9" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="45" t="s">
+      <c r="I9" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="J9" s="45" t="s">
+      <c r="J9" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="K9" s="45" t="s">
+      <c r="K9" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="L9" s="45" t="s">
+      <c r="L9" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="M9" s="45" t="s">
+      <c r="M9" s="44" t="s">
         <v>148</v>
       </c>
-      <c r="N9" s="45" t="s">
+      <c r="N9" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="O9" s="45" t="s">
+      <c r="O9" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="P9" s="45" t="s">
+      <c r="P9" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="Q9" s="45" t="s">
+      <c r="Q9" s="44" t="s">
         <v>105</v>
       </c>
-      <c r="R9" s="45" t="s">
+      <c r="R9" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="S9" s="45" t="s">
+      <c r="S9" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="T9" s="46" t="s">
+      <c r="T9" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="U9" s="46" t="s">
+      <c r="U9" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="V9" s="46" t="s">
+      <c r="V9" s="45" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:22" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{00000000-0002-0000-0D00-000000000000}">
@@ -2721,18 +2753,18 @@
       <selection pane="bottomLeft" activeCell="M29" sqref="A9:M29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" style="7" customWidth="1"/>
     <col min="3" max="4" width="16" style="7" customWidth="1"/>
     <col min="5" max="5" width="18" style="6" customWidth="1"/>
     <col min="6" max="6" width="18" style="8" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.1328125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="34.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
@@ -2743,7 +2775,7 @@
       <c r="F1"/>
       <c r="G1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -2752,7 +2784,7 @@
       <c r="F2"/>
       <c r="G2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>121</v>
       </c>
@@ -2767,7 +2799,7 @@
       <c r="F3"/>
       <c r="G3"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -2782,7 +2814,7 @@
       <c r="F4"/>
       <c r="G4"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>140</v>
       </c>
@@ -2797,7 +2829,7 @@
       <c r="F5"/>
       <c r="G5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>52</v>
       </c>
@@ -2812,7 +2844,7 @@
       <c r="F6"/>
       <c r="G6"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7"/>
@@ -2821,7 +2853,7 @@
       <c r="F7"/>
       <c r="G7"/>
     </row>
-    <row r="8" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -2853,45 +2885,45 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="49"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="49"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="49"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A9" s="48"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" s="48"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11" s="48"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" s="48"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A13" s="48"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
     </row>
   </sheetData>
   <dataValidations count="6">
@@ -2931,17 +2963,17 @@
       <selection pane="bottomLeft" activeCell="L33" sqref="A10:L33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" style="7" customWidth="1"/>
     <col min="3" max="4" width="16" style="7" customWidth="1"/>
     <col min="5" max="5" width="18" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.1328125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="34.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
@@ -2951,7 +2983,7 @@
       <c r="E1"/>
       <c r="F1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -2959,7 +2991,7 @@
       <c r="E2"/>
       <c r="F2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>121</v>
       </c>
@@ -2973,7 +3005,7 @@
       <c r="E3"/>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -2987,7 +3019,7 @@
       <c r="E4"/>
       <c r="F4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>140</v>
       </c>
@@ -3001,7 +3033,7 @@
       <c r="E5"/>
       <c r="F5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>52</v>
       </c>
@@ -3015,7 +3047,7 @@
       <c r="E6"/>
       <c r="F6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>53</v>
       </c>
@@ -3029,7 +3061,7 @@
       <c r="E7"/>
       <c r="F7"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
@@ -3037,7 +3069,7 @@
       <c r="E8"/>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -3066,35 +3098,35 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="49"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="49"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="49"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="48"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" s="48"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" s="48"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" s="48"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" s="48"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
     </row>
   </sheetData>
   <dataValidations count="5">
@@ -3131,22 +3163,22 @@
       <selection pane="bottomLeft" activeCell="M35" sqref="A10:M35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.1328125" customWidth="1"/>
+    <col min="7" max="7" width="34.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>121</v>
       </c>
@@ -3158,7 +3190,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -3170,7 +3202,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>140</v>
       </c>
@@ -3182,7 +3214,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>52</v>
       </c>
@@ -3194,7 +3226,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>53</v>
       </c>
@@ -3206,8 +3238,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -3271,23 +3303,23 @@
       <selection pane="bottomLeft" activeCell="I33" sqref="A9:I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
+    <col min="3" max="3" width="17.86328125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="34.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.1328125" customWidth="1"/>
+    <col min="9" max="9" width="34.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>121</v>
       </c>
@@ -3299,7 +3331,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -3311,7 +3343,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>140</v>
       </c>
@@ -3323,7 +3355,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>52</v>
       </c>
@@ -3335,8 +3367,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="8" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -3400,108 +3432,108 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="43.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.1328125" customWidth="1"/>
+    <col min="2" max="2" width="43.1328125" customWidth="1"/>
     <col min="3" max="16384" width="9" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="58"/>
-    </row>
-    <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="63"/>
+    </row>
+    <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="13"/>
     </row>
-    <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="22" t="s">
         <v>95</v>
       </c>
       <c r="B3" s="12"/>
     </row>
-    <row r="4" spans="1:2" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="14"/>
       <c r="B4" s="18"/>
     </row>
-    <row r="5" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="72" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="19"/>
       <c r="B6" s="19"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="19"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="19"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="19"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="19"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="19"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="19"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="19"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="19"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="19"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="19"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="19"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="19"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="19"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="19"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="19"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" s="19"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" s="19"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" s="19"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" s="19"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" s="19"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" s="19"/>
     </row>
   </sheetData>
@@ -3537,23 +3569,23 @@
       <selection pane="bottomLeft" activeCell="K29" sqref="A10:K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="35.5703125" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.1328125" customWidth="1"/>
+    <col min="7" max="7" width="35.59765625" customWidth="1"/>
+    <col min="8" max="8" width="10.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>121</v>
       </c>
@@ -3565,7 +3597,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -3577,7 +3609,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>140</v>
       </c>
@@ -3589,7 +3621,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>52</v>
       </c>
@@ -3601,7 +3633,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>65</v>
       </c>
@@ -3613,8 +3645,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -3677,24 +3709,24 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.1328125" customWidth="1"/>
+    <col min="8" max="8" width="34.3984375" customWidth="1"/>
+    <col min="9" max="9" width="10.73046875" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>121</v>
       </c>
@@ -3706,7 +3738,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -3718,7 +3750,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>140</v>
       </c>
@@ -3730,7 +3762,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -3742,7 +3774,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
@@ -3754,8 +3786,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -3821,15 +3853,15 @@
       <selection pane="bottomLeft" activeCell="H23" sqref="A10:H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" customWidth="1"/>
+    <col min="2" max="2" width="35.86328125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="36.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="10" t="s">
         <v>72</v>
       </c>
@@ -3837,7 +3869,7 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>121</v>
       </c>
@@ -3848,7 +3880,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -3859,7 +3891,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>80</v>
       </c>
@@ -3870,7 +3902,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>81</v>
       </c>
@@ -3881,7 +3913,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>154</v>
       </c>
@@ -3892,8 +3924,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>75</v>
       </c>
@@ -3948,15 +3980,15 @@
       <selection pane="bottomLeft" activeCell="I37" sqref="A10:I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.86328125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="36.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="10" t="s">
         <v>72</v>
       </c>
@@ -3964,7 +3996,7 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>121</v>
       </c>
@@ -3975,7 +4007,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -3986,7 +4018,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>80</v>
       </c>
@@ -3997,7 +4029,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>82</v>
       </c>
@@ -4008,7 +4040,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>154</v>
       </c>
@@ -4019,8 +4051,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>75</v>
       </c>
@@ -4075,25 +4107,25 @@
       <selection pane="bottomLeft" activeCell="J35" sqref="A10:J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.86328125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="36.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:6" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>121</v>
       </c>
@@ -4104,7 +4136,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -4115,7 +4147,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>84</v>
       </c>
@@ -4126,7 +4158,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>86</v>
       </c>
@@ -4137,7 +4169,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>154</v>
       </c>
@@ -4148,8 +4180,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>75</v>
       </c>
@@ -4207,15 +4239,15 @@
       <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.3984375" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="36.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="10" t="s">
         <v>72</v>
       </c>
@@ -4223,7 +4255,7 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>121</v>
       </c>
@@ -4234,7 +4266,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -4245,7 +4277,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>80</v>
       </c>
@@ -4256,7 +4288,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>81</v>
       </c>
@@ -4267,7 +4299,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>154</v>
       </c>
@@ -4278,8 +4310,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>75</v>
       </c>
@@ -4334,27 +4366,27 @@
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.73046875" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.59765625" customWidth="1"/>
+    <col min="5" max="5" width="33.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:7" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>121</v>
       </c>
@@ -4365,7 +4397,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -4376,7 +4408,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>80</v>
       </c>
@@ -4387,7 +4419,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>81</v>
       </c>
@@ -4398,7 +4430,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>154</v>
       </c>
@@ -4409,8 +4441,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -4470,45 +4502,45 @@
       <selection activeCell="L35" sqref="A6:L35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.1328125" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" customWidth="1"/>
+    <col min="7" max="7" width="26.265625" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="61"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="69"/>
+    </row>
+    <row r="4" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="5" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="23" t="s">
         <v>75</v>
       </c>
@@ -4558,59 +4590,59 @@
       <selection activeCell="K30" sqref="A6:K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="9" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" customWidth="1"/>
-    <col min="11" max="11" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.1328125" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" customWidth="1"/>
+    <col min="3" max="3" width="15.1328125" customWidth="1"/>
+    <col min="5" max="5" width="10.3984375" customWidth="1"/>
+    <col min="6" max="6" width="11.265625" customWidth="1"/>
+    <col min="7" max="7" width="12.1328125" customWidth="1"/>
+    <col min="8" max="9" width="15.73046875" customWidth="1"/>
+    <col min="10" max="10" width="18.1328125" customWidth="1"/>
+    <col min="11" max="11" width="26.265625" customWidth="1"/>
     <col min="12" max="12" width="11" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="13" max="13" width="16.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:13" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="61"/>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="69"/>
+    </row>
+    <row r="4" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="5" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="23" t="s">
         <v>75</v>
       </c>
@@ -4671,42 +4703,42 @@
       <selection activeCell="M34" sqref="A6:M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.86328125" customWidth="1"/>
+    <col min="3" max="3" width="10.1328125" customWidth="1"/>
+    <col min="4" max="4" width="9.73046875" customWidth="1"/>
+    <col min="5" max="5" width="22.265625" customWidth="1"/>
+    <col min="6" max="6" width="11.3984375" customWidth="1"/>
+    <col min="7" max="7" width="15.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
     </row>
-    <row r="3" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="42"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="39"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="41"/>
+    </row>
+    <row r="4" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="5" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="23" t="s">
         <v>98</v>
       </c>
@@ -4748,406 +4780,406 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="31" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="37" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="31" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="23.86328125" bestFit="1" customWidth="1"/>
+    <col min="33" max="37" width="8.3984375" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="14" bestFit="1" customWidth="1"/>
-    <col min="39" max="44" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="58" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="60" max="61" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="44" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="46" max="58" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.73046875" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="7" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="70" max="72" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="25.86328125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="6.3984375" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="70" max="72" width="8.3984375" bestFit="1" customWidth="1"/>
     <col min="73" max="73" width="25" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="9.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="7" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" s="7" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" s="7" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" s="7" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" s="7" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" s="7" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" s="7" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" s="7" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" s="7" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" s="7" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="7" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="7" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="7" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" s="7" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" s="7" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" s="7" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" s="7" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" s="7" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" s="7" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" s="7" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" s="7" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" s="7" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" s="7" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" s="7" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" s="7" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" s="7" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" s="7" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" s="7" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A37" s="7" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38" s="7" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39" s="7" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A40" s="7" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A41" s="7" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42" s="7" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43" s="7" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A44" s="7" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A45" s="7" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A46" s="7" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A47" s="7" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A48" s="7" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A49" s="7" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50" s="7" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A51" s="7" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A52" s="7" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A53" s="7" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A54" s="7" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A55" s="7" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A56" s="7" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A57" s="7" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A58" s="7" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A59" s="7" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A60" s="7" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A61" s="7" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A62" s="7" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A63" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A64" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A65" s="7" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A66" s="7" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A67" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A68" s="7" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A69" s="7" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A70" s="7" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A71" s="7" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A72" s="7" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A73" s="7" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A74" s="7" t="s">
         <v>191</v>
       </c>
@@ -5165,33 +5197,33 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.73046875" customWidth="1"/>
+    <col min="2" max="2" width="37.3984375" customWidth="1"/>
     <col min="3" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="43"/>
+    <col min="5" max="5" width="35.265625" customWidth="1"/>
+    <col min="7" max="7" width="15.73046875" customWidth="1"/>
+    <col min="8" max="8" width="12.3984375" customWidth="1"/>
+    <col min="9" max="16384" width="9.1328125" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:8" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="62" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>253</v>
       </c>
@@ -5203,7 +5235,7 @@
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>136</v>
       </c>
@@ -5213,18 +5245,18 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="6" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="50" t="s">
         <v>250</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="50" t="s">
         <v>251</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="72" t="s">
         <v>115</v>
       </c>
       <c r="E6" s="24" t="s">
@@ -5240,55 +5272,55 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" s="49"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A8" s="49"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A9" s="49"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" s="49"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11" s="49"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5300,7 +5332,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5315,28 +5347,28 @@
       <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.73046875" customWidth="1"/>
+    <col min="2" max="2" width="37.3984375" customWidth="1"/>
+    <col min="3" max="3" width="32.73046875" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="43"/>
+    <col min="5" max="5" width="16.73046875" customWidth="1"/>
+    <col min="6" max="6" width="12.3984375" customWidth="1"/>
+    <col min="7" max="16384" width="9.1328125" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:6" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="62" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>253</v>
       </c>
@@ -5348,7 +5380,7 @@
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>136</v>
       </c>
@@ -5358,12 +5390,12 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="6" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="50" t="s">
         <v>255</v>
       </c>
       <c r="C6" s="24" t="s">
@@ -5379,45 +5411,45 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="49"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="49"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="49"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="49"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="49"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5443,28 +5475,28 @@
       <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.73046875" customWidth="1"/>
+    <col min="2" max="2" width="37.3984375" customWidth="1"/>
+    <col min="3" max="3" width="32.73046875" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="43"/>
+    <col min="5" max="5" width="16.73046875" customWidth="1"/>
+    <col min="6" max="6" width="12.3984375" customWidth="1"/>
+    <col min="7" max="16384" width="9.1328125" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:6" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="62" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>253</v>
       </c>
@@ -5476,7 +5508,7 @@
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>136</v>
       </c>
@@ -5486,12 +5518,12 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="6" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="50" t="s">
         <v>108</v>
       </c>
       <c r="C6" s="24" t="s">
@@ -5507,45 +5539,45 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="49"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="49"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="49"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="49"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="49"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5572,20 +5604,20 @@
       <selection pane="bottomLeft" sqref="A1:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.1328125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.59765625" customWidth="1"/>
+    <col min="7" max="7" width="17.1328125" customWidth="1"/>
+    <col min="8" max="8" width="17.73046875" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="10" t="s">
         <v>259</v>
       </c>
@@ -5593,20 +5625,20 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+    </row>
+    <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="5" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="23" t="s">
         <v>109</v>
       </c>
@@ -5653,21 +5685,21 @@
       <selection pane="bottomLeft" sqref="A1:I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.1328125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.59765625" customWidth="1"/>
+    <col min="7" max="7" width="13.3984375" customWidth="1"/>
+    <col min="8" max="8" width="17.1328125" customWidth="1"/>
+    <col min="9" max="9" width="17.73046875" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
       <c r="A1" s="10" t="s">
         <v>258</v>
       </c>
@@ -5675,21 +5707,21 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+    </row>
+    <row r="4" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="5" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="23" t="s">
         <v>109</v>
       </c>
@@ -5738,38 +5770,38 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="31" customWidth="1"/>
+    <col min="1" max="1" width="18.59765625" style="31" customWidth="1"/>
     <col min="2" max="2" width="52" style="31" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="31"/>
+    <col min="3" max="16384" width="9.1328125" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="30" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:2" s="30" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A1" s="62" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="57"/>
-    </row>
-    <row r="2" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="62"/>
+    </row>
+    <row r="2" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="13"/>
       <c r="B2"/>
     </row>
-    <row r="3" spans="1:2" s="30" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="30" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="37"/>
-    </row>
-    <row r="4" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="36"/>
+    </row>
+    <row r="4" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="14"/>
       <c r="B4" s="18"/>
     </row>
-    <row r="5" spans="1:2" ht="338.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53" t="s">
+    <row r="5" spans="1:2" ht="338.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="51" t="s">
         <v>261</v>
       </c>
-      <c r="B5" s="54"/>
+      <c r="B5" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5787,29 +5819,29 @@
   </sheetPr>
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="75.140625" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
-    <col min="4" max="4" width="43.140625" customWidth="1"/>
+    <col min="1" max="1" width="75.1328125" customWidth="1"/>
+    <col min="2" max="2" width="25.1328125" customWidth="1"/>
+    <col min="3" max="3" width="39.73046875" customWidth="1"/>
+    <col min="4" max="4" width="43.1328125" customWidth="1"/>
     <col min="5" max="16384" width="9" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="63" t="s">
         <v>267</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-    </row>
-    <row r="2" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+    </row>
+    <row r="2" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="22" t="s">
         <v>95</v>
       </c>
@@ -5817,136 +5849,136 @@
       <c r="C2" s="65"/>
       <c r="D2" s="66"/>
     </row>
-    <row r="3" spans="1:4" ht="25.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="25.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="23" t="s">
         <v>268</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="72" t="s">
         <v>269</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="72" t="s">
         <v>270</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="72" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="70" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67"/>
-      <c r="B4" s="68"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="68"/>
-    </row>
-    <row r="5" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="71"/>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="34"/>
-    </row>
-    <row r="6" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="72"/>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="34"/>
-    </row>
-    <row r="7" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="72"/>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="34"/>
-    </row>
-    <row r="8" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="72"/>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="34"/>
-    </row>
-    <row r="9" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="72"/>
-      <c r="B9" s="72"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="34"/>
-    </row>
-    <row r="10" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="72"/>
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="34"/>
-    </row>
-    <row r="11" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="72"/>
-      <c r="B11" s="72"/>
-      <c r="C11" s="72"/>
-      <c r="D11" s="34"/>
-    </row>
-    <row r="12" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="72"/>
-      <c r="B12" s="72"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="34"/>
-    </row>
-    <row r="13" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="72"/>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="34"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="59" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="56"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="57"/>
+    </row>
+    <row r="5" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="60"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="33"/>
+    </row>
+    <row r="6" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="61"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="33"/>
+    </row>
+    <row r="7" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="61"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="33"/>
+    </row>
+    <row r="8" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="61"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="33"/>
+    </row>
+    <row r="9" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="61"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="33"/>
+    </row>
+    <row r="10" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="61"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="33"/>
+    </row>
+    <row r="11" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="61"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="33"/>
+    </row>
+    <row r="12" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="61"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="33"/>
+    </row>
+    <row r="13" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="61"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="33"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="19"/>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
     </row>
-    <row r="15" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15" s="19"/>
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
     </row>
-    <row r="16" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A16" s="19"/>
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
     </row>
-    <row r="17" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A17" s="19"/>
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
     </row>
-    <row r="18" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="19"/>
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
     </row>
-    <row r="19" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A19" s="19"/>
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
     </row>
-    <row r="20" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="19"/>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
     </row>
-    <row r="21" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" s="19"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
     </row>
-    <row r="22" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A22" s="19"/>
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
     </row>
-    <row r="23" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A23" s="19"/>
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
     </row>
-    <row r="24" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A24" s="19"/>
       <c r="B24" s="19"/>
       <c r="C24" s="19"/>
     </row>
-    <row r="25" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A25" s="19"/>
       <c r="B25" s="19"/>
       <c r="C25" s="19"/>
@@ -5968,35 +6000,35 @@
   </sheetPr>
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.73046875" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="39"/>
+    <col min="4" max="4" width="16.1328125" customWidth="1"/>
+    <col min="5" max="5" width="36.1328125" customWidth="1"/>
+    <col min="6" max="6" width="9.73046875" customWidth="1"/>
+    <col min="7" max="7" width="10.3984375" customWidth="1"/>
+    <col min="8" max="16384" width="9.1328125" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:7" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -6005,7 +6037,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>121</v>
       </c>
@@ -6020,7 +6052,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -6035,12 +6067,12 @@
       <c r="F4" s="15"/>
       <c r="G4" s="16"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>159</v>
+        <v>25</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -6050,12 +6082,12 @@
       <c r="F5" s="15"/>
       <c r="G5" s="16"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>160</v>
+        <v>25</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>24</v>
@@ -6065,7 +6097,7 @@
       <c r="F6" s="15"/>
       <c r="G6" s="16"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="20"/>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -6074,7 +6106,7 @@
       <c r="F7" s="20"/>
       <c r="G7" s="21"/>
     </row>
-    <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -6128,35 +6160,35 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.86328125" customWidth="1"/>
+    <col min="2" max="2" width="22.86328125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="34.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.1328125" customWidth="1"/>
+    <col min="6" max="6" width="34.3984375" customWidth="1"/>
     <col min="7" max="7" width="9"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="38"/>
+    <col min="8" max="8" width="10.1328125" customWidth="1"/>
+    <col min="9" max="16384" width="9.1328125" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:8" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>121</v>
       </c>
@@ -6168,7 +6200,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -6180,7 +6212,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>125</v>
       </c>
@@ -6192,7 +6224,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>84</v>
       </c>
@@ -6204,7 +6236,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -6216,10 +6248,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="23" t="s">
         <v>4</v>
       </c>
@@ -6282,34 +6314,34 @@
       <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.73046875" customWidth="1"/>
+    <col min="2" max="2" width="20.265625" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="25"/>
+    <col min="5" max="5" width="16.1328125" customWidth="1"/>
+    <col min="6" max="6" width="14.3984375" customWidth="1"/>
+    <col min="7" max="7" width="31.3984375" customWidth="1"/>
+    <col min="8" max="8" width="11.1328125" customWidth="1"/>
+    <col min="9" max="9" width="11.265625" customWidth="1"/>
+    <col min="10" max="16384" width="9.1328125" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>121</v>
       </c>
@@ -6320,7 +6352,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -6331,7 +6363,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -6342,7 +6374,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -6353,8 +6385,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="8" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -6418,34 +6450,34 @@
       <selection pane="bottomLeft" activeCell="G32" sqref="A9:G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="27"/>
+    <col min="5" max="5" width="16.1328125" customWidth="1"/>
+    <col min="6" max="6" width="11.1328125" customWidth="1"/>
+    <col min="7" max="7" width="34.3984375" customWidth="1"/>
+    <col min="8" max="8" width="10.73046875" customWidth="1"/>
+    <col min="9" max="9" width="15.1328125" customWidth="1"/>
+    <col min="10" max="16384" width="9.1328125" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>121</v>
       </c>
@@ -6457,7 +6489,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -6469,7 +6501,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -6481,7 +6513,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -6493,8 +6525,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="8" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
@@ -6558,34 +6590,34 @@
       <selection pane="bottomLeft" activeCell="H27" sqref="A11:H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1"/>
-    <col min="9" max="9" width="34.42578125" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
+    <col min="5" max="7" width="16.1328125" customWidth="1"/>
+    <col min="8" max="8" width="11.86328125" customWidth="1"/>
+    <col min="9" max="9" width="34.3984375" customWidth="1"/>
+    <col min="11" max="11" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:11" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>121</v>
       </c>
@@ -6597,7 +6629,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -6609,7 +6641,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -6621,7 +6653,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -6633,7 +6665,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -6645,7 +6677,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -6657,10 +6689,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="23" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Font changes and hover comments
</commit_message>
<xml_diff>
--- a/XML/Atomistic-Class1/WebFF-Class1-DataTemplate.xlsx
+++ b/XML/Atomistic-Class1/WebFF-Class1-DataTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Projects\WebFF-Documentation\XML\Atomistic-Class1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A416E45-7F2F-485D-B64F-77E29BA877EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312CEDDE-3F77-432A-92A3-B628D44815F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" firstSheet="28" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="44" r:id="rId1"/>
@@ -70,7 +70,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional entry, not required
 </t>
@@ -84,7 +84,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional entry, not required
 </t>
@@ -98,7 +98,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional entry, not required
 </t>
@@ -123,7 +123,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -137,7 +137,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -151,7 +151,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -165,7 +165,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -178,7 +178,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -192,7 +192,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -206,7 +206,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -231,7 +231,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -245,7 +245,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -259,7 +259,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -273,7 +273,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -287,7 +287,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -300,7 +300,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -314,7 +314,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -328,7 +328,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -353,7 +353,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -367,7 +367,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -381,7 +381,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -395,7 +395,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -408,7 +408,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -422,7 +422,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -436,7 +436,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -461,7 +461,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -475,7 +475,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -489,7 +489,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -503,7 +503,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -516,7 +516,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -530,7 +530,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -544,7 +544,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -569,7 +569,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -583,7 +583,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -597,7 +597,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -611,7 +611,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -625,7 +625,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -638,7 +638,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -652,7 +652,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -666,7 +666,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -691,7 +691,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -705,7 +705,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -719,7 +719,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -733,7 +733,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -746,7 +746,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -760,7 +760,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -774,7 +774,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -799,7 +799,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -813,7 +813,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -827,7 +827,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -841,7 +841,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -855,7 +855,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -868,7 +868,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -882,7 +882,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -896,7 +896,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -921,7 +921,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -935,7 +935,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -949,7 +949,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -963,7 +963,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -977,7 +977,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -990,7 +990,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1004,7 +1004,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1018,7 +1018,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1043,7 +1043,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1057,7 +1057,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1071,7 +1071,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1085,7 +1085,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1098,7 +1098,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1112,7 +1112,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1126,7 +1126,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1151,7 +1151,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1165,7 +1165,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1179,7 +1179,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1193,7 +1193,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1207,7 +1207,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1220,7 +1220,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1234,7 +1234,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1248,7 +1248,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1272,7 +1272,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional entry, not required
 </t>
@@ -1297,7 +1297,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1311,7 +1311,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1325,7 +1325,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1339,7 +1339,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1353,7 +1353,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1366,7 +1366,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1380,7 +1380,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1394,7 +1394,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1419,7 +1419,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1433,7 +1433,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1447,7 +1447,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1461,7 +1461,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1475,7 +1475,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1488,7 +1488,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1502,7 +1502,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1516,7 +1516,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1541,7 +1541,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1555,7 +1555,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1569,7 +1569,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1583,7 +1583,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1597,7 +1597,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1610,7 +1610,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1624,7 +1624,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1638,7 +1638,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1663,7 +1663,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1677,7 +1677,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1691,7 +1691,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1705,7 +1705,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1719,7 +1719,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1732,7 +1732,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1746,7 +1746,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1760,7 +1760,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1785,7 +1785,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1799,7 +1799,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1813,7 +1813,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1827,7 +1827,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1841,7 +1841,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1854,7 +1854,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1868,7 +1868,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1882,7 +1882,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1907,7 +1907,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1921,7 +1921,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1935,7 +1935,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1949,7 +1949,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1963,7 +1963,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -1976,7 +1976,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -1990,7 +1990,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2004,7 +2004,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2028,7 +2028,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2042,7 +2042,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2056,7 +2056,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2080,7 +2080,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2094,7 +2094,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2108,7 +2108,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2132,7 +2132,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2146,7 +2146,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2160,7 +2160,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2185,7 +2185,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -2199,7 +2199,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -2213,7 +2213,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Optional entry, not required</t>
         </r>
@@ -2226,7 +2226,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2240,7 +2240,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2254,7 +2254,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2268,7 +2268,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2292,7 +2292,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional entry, not required
 </t>
@@ -2306,7 +2306,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional entry, not required
 </t>
@@ -2320,7 +2320,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional entry, not required
 </t>
@@ -2345,7 +2345,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -2359,7 +2359,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -2372,7 +2372,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2386,7 +2386,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2400,7 +2400,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2414,7 +2414,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2439,7 +2439,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -2453,7 +2453,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -2466,7 +2466,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2480,7 +2480,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2494,7 +2494,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2508,7 +2508,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2899,7 +2899,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -2913,7 +2913,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -2927,7 +2927,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -2941,7 +2941,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -2954,7 +2954,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2968,7 +2968,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -2982,7 +2982,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -3007,7 +3007,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -3021,7 +3021,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -3035,7 +3035,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -3049,7 +3049,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -3063,7 +3063,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -3076,7 +3076,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -3090,7 +3090,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -3104,7 +3104,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -3129,7 +3129,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -3143,7 +3143,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -3157,7 +3157,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -3171,7 +3171,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -3184,7 +3184,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -3198,7 +3198,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -3212,7 +3212,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -3226,7 +3226,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -3251,7 +3251,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -3265,7 +3265,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -3279,7 +3279,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -3293,7 +3293,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -3306,7 +3306,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -3320,7 +3320,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -3334,7 +3334,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -3348,7 +3348,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -3373,7 +3373,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -3387,7 +3387,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -3401,7 +3401,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -3415,7 +3415,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -3429,7 +3429,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -3443,7 +3443,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -3456,7 +3456,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -3470,7 +3470,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -3484,7 +3484,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -3498,7 +3498,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -3523,7 +3523,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -3537,7 +3537,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -3551,7 +3551,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -3565,7 +3565,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -3579,7 +3579,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
@@ -3592,7 +3592,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -3606,7 +3606,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -3620,7 +3620,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Optional attribute data, not required
 </t>
@@ -4424,7 +4424,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4505,7 +4505,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -4520,29 +4520,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -4778,7 +4756,7 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4884,6 +4862,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4910,10 +4891,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -5281,10 +5258,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="30" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="61"/>
+      <c r="B1" s="62"/>
     </row>
     <row r="2" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
@@ -6990,10 +6967,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="62"/>
+      <c r="B1" s="63"/>
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
@@ -7668,14 +7645,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -7930,15 +7907,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -8067,32 +8044,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="69"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8162,40 +8139,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="67"/>
-      <c r="M3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="69"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8271,15 +8248,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
     </row>
@@ -8770,16 +8747,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -8918,14 +8895,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -9047,14 +9024,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -9190,13 +9167,13 @@
       <c r="A3" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -9244,7 +9221,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9273,14 +9250,14 @@
       <c r="A3" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -9290,25 +9267,25 @@
       <c r="B5" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="70" t="s">
+      <c r="C5" s="60" t="s">
         <v>117</v>
       </c>
-      <c r="D5" s="70" t="s">
+      <c r="D5" s="60" t="s">
         <v>116</v>
       </c>
-      <c r="E5" s="70" t="s">
+      <c r="E5" s="60" t="s">
         <v>115</v>
       </c>
-      <c r="F5" s="70" t="s">
+      <c r="F5" s="60" t="s">
         <v>114</v>
       </c>
-      <c r="G5" s="70" t="s">
+      <c r="G5" s="60" t="s">
         <v>113</v>
       </c>
-      <c r="H5" s="70" t="s">
+      <c r="H5" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="I5" s="70" t="s">
+      <c r="I5" s="60" t="s">
         <v>111</v>
       </c>
     </row>
@@ -9329,7 +9306,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -9341,10 +9318,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="30" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="61"/>
+      <c r="B1" s="62"/>
     </row>
     <row r="2" spans="1:2" s="30" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
@@ -9361,7 +9338,7 @@
       <c r="B4" s="18"/>
     </row>
     <row r="5" spans="1:2" ht="338.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="61" t="s">
         <v>246</v>
       </c>
       <c r="B5" s="49"/>
@@ -9398,20 +9375,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="63" t="s">
         <v>252</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="66"/>
     </row>
     <row r="3" spans="1:4" ht="25.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
@@ -9583,15 +9560,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
@@ -9743,16 +9720,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -9896,17 +9873,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -10013,7 +9990,7 @@
   </sheetPr>
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F8" sqref="F8:I8"/>
     </sheetView>
@@ -10033,17 +10010,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -10172,19 +10149,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">

</xml_diff>